<commit_message>
worked on auto grapher, still trash, dont use
</commit_message>
<xml_diff>
--- a/Smutans/TestData1.xlsx
+++ b/Smutans/TestData1.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andres\Documents\HTML\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Andres\Documents\HTML\Smutans\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC397DB7-8FFF-49E7-90AD-720562EACAC0}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8505"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -336,16 +335,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>10</v>
       </c>
@@ -383,7 +382,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>50</v>
       </c>
@@ -421,7 +420,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>24</v>
       </c>
@@ -459,7 +458,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>12</v>
       </c>
@@ -489,9 +488,6 @@
       </c>
       <c r="J4">
         <v>14</v>
-      </c>
-      <c r="K4">
-        <v>56</v>
       </c>
       <c r="L4">
         <v>32</v>

</xml_diff>